<commit_message>
novo seed arrumado com novos tags de paid ou em aberto
</commit_message>
<xml_diff>
--- a/lib/xlsx_reader/operacoes2.xlsx
+++ b/lib/xlsx_reader/operacoes2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="24240" windowHeight="13500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="RelatorioOperacao_completo" sheetId="1" r:id="rId1"/>
@@ -4395,7 +4395,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4556,6 +4556,14 @@
       <b/>
       <sz val="7.5"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5024,14 +5032,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -5388,13 +5396,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1454"/>
+  <dimension ref="A1:T1454"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="O141" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="R141" sqref="R141"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5408,7 +5416,7 @@
     <col min="20" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16" customHeight="1">
+    <row r="1" spans="1:20" ht="16" customHeight="1">
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
@@ -5430,17 +5438,67 @@
       <c r="R1" s="9"/>
       <c r="S1" s="13"/>
     </row>
-    <row r="2" spans="1:19">
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
-      <c r="S2" s="14"/>
-    </row>
-    <row r="3" spans="1:19">
+    <row r="2" spans="1:20" ht="21">
+      <c r="A2" s="18">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20">
+        <v>2</v>
+      </c>
+      <c r="D2" s="20">
+        <v>3</v>
+      </c>
+      <c r="E2" s="20">
+        <v>4</v>
+      </c>
+      <c r="F2" s="20">
+        <v>5</v>
+      </c>
+      <c r="G2" s="20">
+        <v>6</v>
+      </c>
+      <c r="H2" s="18">
+        <v>7</v>
+      </c>
+      <c r="I2" s="19">
+        <v>8</v>
+      </c>
+      <c r="J2" s="20">
+        <v>9</v>
+      </c>
+      <c r="K2" s="20">
+        <v>10</v>
+      </c>
+      <c r="L2" s="20">
+        <v>11</v>
+      </c>
+      <c r="M2" s="20">
+        <v>12</v>
+      </c>
+      <c r="N2" s="20">
+        <v>13</v>
+      </c>
+      <c r="O2" s="18">
+        <v>14</v>
+      </c>
+      <c r="P2" s="19">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="20">
+        <v>16</v>
+      </c>
+      <c r="R2" s="20">
+        <v>17</v>
+      </c>
+      <c r="S2" s="20">
+        <v>18</v>
+      </c>
+      <c r="T2" s="20"/>
+    </row>
+    <row r="3" spans="1:20">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -5496,7 +5554,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>19</v>
@@ -5527,7 +5585,7 @@
       </c>
       <c r="S4" s="14"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -5586,7 +5644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" s="1">
         <f>IF(ISBLANK(B6),A5,B6)</f>
         <v>1</v>
@@ -5621,7 +5679,7 @@
       </c>
       <c r="S6" s="14"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20">
       <c r="A7" s="1">
         <f t="shared" ref="A7:A70" si="0">IF(ISBLANK(B7),A6,B7)</f>
         <v>2</v>
@@ -5681,7 +5739,7 @@
         <v>1026.6400000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:20">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -5716,7 +5774,7 @@
       </c>
       <c r="S8" s="14"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:20">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -5751,7 +5809,7 @@
       </c>
       <c r="S9" s="14"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:20">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -5786,7 +5844,7 @@
       </c>
       <c r="S10" s="14"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:20">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5846,7 +5904,7 @@
         <v>60.85</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:20">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5881,7 +5939,7 @@
       </c>
       <c r="S12" s="14"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:20">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5916,7 +5974,7 @@
       </c>
       <c r="S13" s="14"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:20">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5976,7 +6034,7 @@
         <v>167.97</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:20">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6011,7 +6069,7 @@
       </c>
       <c r="S15" s="14"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -64453,9 +64511,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A3:S1454"/>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>

</xml_diff>